<commit_message>
Updated Task, Schedule Metrics and risk
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Risks/Risk Management.xlsx
+++ b/Documents/Project Management/Risks/Risk Management.xlsx
@@ -83,17 +83,7 @@
     <t xml:space="preserve">Project will be potentially delayed due to incorrect estimates. The quality of the system might not be as satisfactory as there might be more bugs. </t>
   </si>
   <si>
-    <t>Lead developer to organise lessons for team members to learn. Project Manager to allocate more time to this task.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Servers – Client is unable to provide access to local server during development phase due to IT security concerns </t>
-  </si>
-  <si>
     <t xml:space="preserve">Application may not be compatible with the client’s server. </t>
-  </si>
-  <si>
-    <t>Team to deploy on team’s local server during development phase. 
-Team to know the client’s server’s specifications and ensure that the local server used is close to the client’s local server.</t>
   </si>
   <si>
     <t>Project Management Risks</t>
@@ -134,6 +124,16 @@
   </si>
   <si>
     <t xml:space="preserve">PM should spot and ensure any members who are quiet during the meeting. PM could also go a round table approach whereby everyone has to voice out at least once for a certain idea. </t>
+  </si>
+  <si>
+    <t>Lead developer will research and dicuss with the team. Project Manager to allocate more time to this task.</t>
+  </si>
+  <si>
+    <t>Servers – Client is unable to provide access to local server during development phase</t>
+  </si>
+  <si>
+    <t>Team to deploy on OpenShift during development phase. 
+Team to know the client's server's specifications and research on deployment prior to deployment to client's server.</t>
   </si>
 </sst>
 </file>
@@ -206,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -307,12 +307,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -332,9 +345,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -344,26 +354,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -381,6 +427,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1219200" y="1514475"/>
+          <a:ext cx="3933825" cy="1495425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -673,113 +779,113 @@
   <dimension ref="B1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B15" sqref="B15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="24.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" style="13" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="2:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="95.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" ht="95.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="19" t="s">
+      <c r="D5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="9" t="s">
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="2:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -799,11 +905,11 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="108.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="19" t="s">
-        <v>27</v>
+      <c r="B9" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>3</v>
@@ -815,15 +921,15 @@
         <v>6</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="108.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="19" t="s">
-        <v>30</v>
+      <c r="B10" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>3</v>
@@ -835,15 +941,15 @@
         <v>6</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="122.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="19" t="s">
-        <v>33</v>
+      <c r="B11" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>3</v>
@@ -855,7 +961,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -863,17 +969,17 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
+      <c r="B13" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="2:7" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -893,11 +999,11 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="19" t="s">
-        <v>36</v>
+      <c r="B15" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>3</v>
@@ -909,7 +1015,7 @@
         <v>6</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
@@ -931,54 +1037,61 @@
     <mergeCell ref="B7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="C2:F6"/>
+      <selection activeCell="J11" sqref="J11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="59.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" style="19" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
+    </row>
+    <row r="3" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="4" t="s">
@@ -994,7 +1107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="4" t="s">
@@ -1010,7 +1123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
@@ -1026,80 +1139,84 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="J8" s="25" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K8" s="26"/>
+    </row>
+    <row r="9" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="J9" s="27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="J10" s="27" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K10" s="28"/>
+    </row>
+    <row r="11" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="J11" s="29" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="K11" s="30"/>
+    </row>
+    <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1107,9 +1224,14 @@
       <c r="E14" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="D2:F2"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>